<commit_message>
inicio proyecto carrito de compras
</commit_message>
<xml_diff>
--- a/reporte ventas.xlsx
+++ b/reporte ventas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sebastian\programacion22-23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008B69EB-E81A-49AD-86F9-2B53E738E603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100B278B-41E2-470D-9F80-5CDDEAA2F90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="73">
   <si>
     <t>Reporte de Ventas</t>
   </si>
@@ -253,6 +253,9 @@
   <si>
     <t>Semana 19 Junio - 24 de Junio</t>
   </si>
+  <si>
+    <t>Semana 26 Junio - 1 de Julio</t>
+  </si>
 </sst>
 </file>
 
@@ -421,11 +424,11 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -700,10 +703,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3168</c:v>
+                  <c:v>3213</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4033</c:v>
+                  <c:v>4057</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>656</c:v>
@@ -5135,8 +5138,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="B5:F226" totalsRowShown="0">
-  <autoFilter ref="B5:F226" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="B5:F229" totalsRowShown="0">
+  <autoFilter ref="B5:F229" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0">
       <filters>
         <dateGroupItem year="2023" month="6" dateTimeGrouping="month"/>
@@ -5487,10 +5490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:W226"/>
+  <dimension ref="B2:W229"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A209" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B227" sqref="B227"/>
+      <selection activeCell="O216" sqref="O216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5506,27 +5509,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="H2" s="20" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="H2" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
@@ -5544,21 +5547,21 @@
       </c>
     </row>
     <row r="4" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="2">
         <f xml:space="preserve"> SUM(Tabla1[sebastian])</f>
-        <v>3168</v>
+        <v>3213</v>
       </c>
       <c r="J4" s="2">
         <f xml:space="preserve"> SUM(Tabla1[angelica])</f>
-        <v>4033</v>
+        <v>4057</v>
       </c>
       <c r="K4" s="2">
         <f xml:space="preserve"> SUM(Tabla1[alejandro])</f>
@@ -5566,7 +5569,7 @@
       </c>
       <c r="L4" s="14">
         <f xml:space="preserve"> SUM(Tabla1[valor venta])</f>
-        <v>32613600</v>
+        <v>32899500</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -5598,13 +5601,13 @@
       <c r="F6" s="16">
         <v>147600</v>
       </c>
-      <c r="I6" s="20" t="s">
+      <c r="I6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
     </row>
     <row r="7" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -5686,13 +5689,13 @@
       <c r="F10" s="16">
         <v>26400</v>
       </c>
-      <c r="I10" s="20" t="s">
+      <c r="I10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
     </row>
     <row r="11" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -5735,11 +5738,11 @@
       </c>
       <c r="J12" s="2">
         <f xml:space="preserve"> SUM(Tabla1[sebastian])</f>
-        <v>3168</v>
+        <v>3213</v>
       </c>
       <c r="K12" s="2">
         <f xml:space="preserve"> SUM(Tabla1[angelica])</f>
-        <v>4033</v>
+        <v>4057</v>
       </c>
       <c r="L12" s="2">
         <f xml:space="preserve"> SUM(Tabla1[alejandro])</f>
@@ -5747,7 +5750,7 @@
       </c>
       <c r="M12" s="2">
         <f>SUM(J12:L12)</f>
-        <v>7857</v>
+        <v>7926</v>
       </c>
     </row>
     <row r="13" spans="2:14" hidden="1" x14ac:dyDescent="0.25">
@@ -5816,13 +5819,13 @@
       <c r="F18" s="16">
         <v>13200</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
     </row>
     <row r="19" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
@@ -6000,16 +6003,16 @@
       <c r="F31" s="16">
         <v>270600</v>
       </c>
-      <c r="I31" s="20" t="s">
+      <c r="I31" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
     </row>
     <row r="32" spans="2:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
@@ -6116,16 +6119,16 @@
       <c r="F35" s="16">
         <v>57200</v>
       </c>
-      <c r="I35" s="20" t="s">
+      <c r="I35" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
       <c r="V35" s="7"/>
       <c r="W35" s="14">
         <v>65000</v>
@@ -6240,16 +6243,16 @@
       <c r="F39" s="16">
         <v>155800</v>
       </c>
-      <c r="I39" s="20" t="s">
+      <c r="I39" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
       <c r="V39" s="11"/>
       <c r="W39" s="14">
         <v>52000</v>
@@ -6360,16 +6363,16 @@
       <c r="F43" s="16">
         <v>176300</v>
       </c>
-      <c r="I43" s="20" t="s">
+      <c r="I43" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
     </row>
     <row r="44" spans="2:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
@@ -6468,13 +6471,13 @@
       <c r="F47" s="16">
         <v>105600</v>
       </c>
-      <c r="I47" s="20" t="s">
+      <c r="I47" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
     </row>
     <row r="48" spans="2:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
@@ -6938,16 +6941,16 @@
       <c r="F86" s="16">
         <v>463300</v>
       </c>
-      <c r="H86" s="20" t="s">
+      <c r="H86" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I86" s="20"/>
-      <c r="J86" s="20"/>
-      <c r="K86" s="20"/>
-      <c r="L86" s="20"/>
-      <c r="M86" s="20"/>
-      <c r="N86" s="20"/>
-      <c r="O86" s="20"/>
+      <c r="I86" s="19"/>
+      <c r="J86" s="19"/>
+      <c r="K86" s="19"/>
+      <c r="L86" s="19"/>
+      <c r="M86" s="19"/>
+      <c r="N86" s="19"/>
+      <c r="O86" s="19"/>
     </row>
     <row r="87" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
@@ -7046,16 +7049,16 @@
       <c r="F90" s="16">
         <v>147600</v>
       </c>
-      <c r="H90" s="20" t="s">
+      <c r="H90" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="I90" s="20"/>
-      <c r="J90" s="20"/>
-      <c r="K90" s="20"/>
-      <c r="L90" s="20"/>
-      <c r="M90" s="20"/>
-      <c r="N90" s="20"/>
-      <c r="O90" s="20"/>
+      <c r="I90" s="19"/>
+      <c r="J90" s="19"/>
+      <c r="K90" s="19"/>
+      <c r="L90" s="19"/>
+      <c r="M90" s="19"/>
+      <c r="N90" s="19"/>
+      <c r="O90" s="19"/>
     </row>
     <row r="91" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B91" s="1">
@@ -7154,16 +7157,16 @@
       <c r="F94" s="16">
         <v>101200</v>
       </c>
-      <c r="H94" s="20" t="s">
+      <c r="H94" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="I94" s="20"/>
-      <c r="J94" s="20"/>
-      <c r="K94" s="20"/>
-      <c r="L94" s="20"/>
-      <c r="M94" s="20"/>
-      <c r="N94" s="20"/>
-      <c r="O94" s="20"/>
+      <c r="I94" s="19"/>
+      <c r="J94" s="19"/>
+      <c r="K94" s="19"/>
+      <c r="L94" s="19"/>
+      <c r="M94" s="19"/>
+      <c r="N94" s="19"/>
+      <c r="O94" s="19"/>
     </row>
     <row r="95" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
@@ -7262,16 +7265,16 @@
       <c r="F98" s="16">
         <v>240000</v>
       </c>
-      <c r="H98" s="20" t="s">
+      <c r="H98" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="I98" s="20"/>
-      <c r="J98" s="20"/>
-      <c r="K98" s="20"/>
-      <c r="L98" s="20"/>
-      <c r="M98" s="20"/>
-      <c r="N98" s="20"/>
-      <c r="O98" s="20"/>
+      <c r="I98" s="19"/>
+      <c r="J98" s="19"/>
+      <c r="K98" s="19"/>
+      <c r="L98" s="19"/>
+      <c r="M98" s="19"/>
+      <c r="N98" s="19"/>
+      <c r="O98" s="19"/>
     </row>
     <row r="99" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B99" s="1">
@@ -7370,13 +7373,13 @@
       <c r="F102" s="16">
         <v>105600</v>
       </c>
-      <c r="H102" s="20" t="s">
+      <c r="H102" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="I102" s="20"/>
-      <c r="J102" s="20"/>
-      <c r="K102" s="20"/>
-      <c r="L102" s="20"/>
+      <c r="I102" s="19"/>
+      <c r="J102" s="19"/>
+      <c r="K102" s="19"/>
+      <c r="L102" s="19"/>
     </row>
     <row r="103" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B103" s="1">
@@ -7587,16 +7590,16 @@
       <c r="F118" s="16">
         <v>107200</v>
       </c>
-      <c r="H118" s="20" t="s">
+      <c r="H118" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="I118" s="20"/>
-      <c r="J118" s="20"/>
-      <c r="K118" s="20"/>
-      <c r="L118" s="20"/>
-      <c r="M118" s="20"/>
-      <c r="N118" s="20"/>
-      <c r="O118" s="20"/>
+      <c r="I118" s="19"/>
+      <c r="J118" s="19"/>
+      <c r="K118" s="19"/>
+      <c r="L118" s="19"/>
+      <c r="M118" s="19"/>
+      <c r="N118" s="19"/>
+      <c r="O118" s="19"/>
     </row>
     <row r="119" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B119" s="1">
@@ -7695,16 +7698,16 @@
       <c r="F122" s="16">
         <v>147600</v>
       </c>
-      <c r="H122" s="20" t="s">
+      <c r="H122" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="I122" s="20"/>
-      <c r="J122" s="20"/>
-      <c r="K122" s="20"/>
-      <c r="L122" s="20"/>
-      <c r="M122" s="20"/>
-      <c r="N122" s="20"/>
-      <c r="O122" s="20"/>
+      <c r="I122" s="19"/>
+      <c r="J122" s="19"/>
+      <c r="K122" s="19"/>
+      <c r="L122" s="19"/>
+      <c r="M122" s="19"/>
+      <c r="N122" s="19"/>
+      <c r="O122" s="19"/>
     </row>
     <row r="123" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B123" s="1">
@@ -7803,16 +7806,16 @@
       <c r="F126" s="16">
         <v>123200</v>
       </c>
-      <c r="H126" s="20" t="s">
+      <c r="H126" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="I126" s="20"/>
-      <c r="J126" s="20"/>
-      <c r="K126" s="20"/>
-      <c r="L126" s="20"/>
-      <c r="M126" s="20"/>
-      <c r="N126" s="20"/>
-      <c r="O126" s="20"/>
+      <c r="I126" s="19"/>
+      <c r="J126" s="19"/>
+      <c r="K126" s="19"/>
+      <c r="L126" s="19"/>
+      <c r="M126" s="19"/>
+      <c r="N126" s="19"/>
+      <c r="O126" s="19"/>
     </row>
     <row r="127" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B127" s="1">
@@ -7911,16 +7914,16 @@
       <c r="F130" s="16">
         <v>192000</v>
       </c>
-      <c r="H130" s="20" t="s">
+      <c r="H130" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="I130" s="20"/>
-      <c r="J130" s="20"/>
-      <c r="K130" s="20"/>
-      <c r="L130" s="20"/>
-      <c r="M130" s="20"/>
-      <c r="N130" s="20"/>
-      <c r="O130" s="20"/>
+      <c r="I130" s="19"/>
+      <c r="J130" s="19"/>
+      <c r="K130" s="19"/>
+      <c r="L130" s="19"/>
+      <c r="M130" s="19"/>
+      <c r="N130" s="19"/>
+      <c r="O130" s="19"/>
     </row>
     <row r="131" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B131" s="1">
@@ -8019,13 +8022,13 @@
       <c r="F134" s="16">
         <v>147600</v>
       </c>
-      <c r="H134" s="20" t="s">
+      <c r="H134" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="I134" s="20"/>
-      <c r="J134" s="20"/>
-      <c r="K134" s="20"/>
-      <c r="L134" s="20"/>
+      <c r="I134" s="19"/>
+      <c r="J134" s="19"/>
+      <c r="K134" s="19"/>
+      <c r="L134" s="19"/>
     </row>
     <row r="135" spans="2:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="B135" s="1">
@@ -8720,16 +8723,16 @@
       <c r="F194" s="16">
         <v>288000</v>
       </c>
-      <c r="H194" s="20" t="s">
+      <c r="H194" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="I194" s="20"/>
-      <c r="J194" s="20"/>
-      <c r="K194" s="20"/>
-      <c r="L194" s="20"/>
-      <c r="M194" s="20"/>
-      <c r="N194" s="20"/>
-      <c r="O194" s="20"/>
+      <c r="I194" s="19"/>
+      <c r="J194" s="19"/>
+      <c r="K194" s="19"/>
+      <c r="L194" s="19"/>
+      <c r="M194" s="19"/>
+      <c r="N194" s="19"/>
+      <c r="O194" s="19"/>
     </row>
     <row r="195" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B195" s="1">
@@ -8839,16 +8842,16 @@
       <c r="F199" s="16">
         <v>384000</v>
       </c>
-      <c r="H199" s="20" t="s">
+      <c r="H199" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="I199" s="20"/>
-      <c r="J199" s="20"/>
-      <c r="K199" s="20"/>
-      <c r="L199" s="20"/>
-      <c r="M199" s="20"/>
-      <c r="N199" s="20"/>
-      <c r="O199" s="20"/>
+      <c r="I199" s="19"/>
+      <c r="J199" s="19"/>
+      <c r="K199" s="19"/>
+      <c r="L199" s="19"/>
+      <c r="M199" s="19"/>
+      <c r="N199" s="19"/>
+      <c r="O199" s="19"/>
     </row>
     <row r="200" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B200" s="1">
@@ -8958,16 +8961,16 @@
       <c r="F204" s="16">
         <v>144000</v>
       </c>
-      <c r="H204" s="20" t="s">
+      <c r="H204" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="I204" s="20"/>
-      <c r="J204" s="20"/>
-      <c r="K204" s="20"/>
-      <c r="L204" s="20"/>
-      <c r="M204" s="20"/>
-      <c r="N204" s="20"/>
-      <c r="O204" s="20"/>
+      <c r="I204" s="19"/>
+      <c r="J204" s="19"/>
+      <c r="K204" s="19"/>
+      <c r="L204" s="19"/>
+      <c r="M204" s="19"/>
+      <c r="N204" s="19"/>
+      <c r="O204" s="19"/>
     </row>
     <row r="205" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B205" s="1">
@@ -9077,16 +9080,16 @@
       <c r="F209" s="16">
         <v>74000</v>
       </c>
-      <c r="H209" s="20" t="s">
+      <c r="H209" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="I209" s="20"/>
-      <c r="J209" s="20"/>
-      <c r="K209" s="20"/>
-      <c r="L209" s="20"/>
-      <c r="M209" s="20"/>
-      <c r="N209" s="20"/>
-      <c r="O209" s="20"/>
+      <c r="I209" s="19"/>
+      <c r="J209" s="19"/>
+      <c r="K209" s="19"/>
+      <c r="L209" s="19"/>
+      <c r="M209" s="19"/>
+      <c r="N209" s="19"/>
+      <c r="O209" s="19"/>
     </row>
     <row r="210" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B210" s="1">
@@ -9196,6 +9199,16 @@
       <c r="F214" s="16">
         <v>144000</v>
       </c>
+      <c r="H214" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="I214" s="19"/>
+      <c r="J214" s="19"/>
+      <c r="K214" s="19"/>
+      <c r="L214" s="19"/>
+      <c r="M214" s="19"/>
+      <c r="N214" s="19"/>
+      <c r="O214" s="19"/>
     </row>
     <row r="215" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B215" s="1">
@@ -9207,6 +9220,30 @@
       <c r="F215" s="16">
         <v>77400</v>
       </c>
+      <c r="H215" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I215" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J215" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K215" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L215" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M215" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N215" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O215" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="216" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B216" s="1">
@@ -9218,6 +9255,36 @@
       <c r="F216" s="16">
         <v>144000</v>
       </c>
+      <c r="H216" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I216" s="2">
+        <f>SUM($C224:$C229)</f>
+        <v>49</v>
+      </c>
+      <c r="J216" s="2">
+        <f>SUM(D224:D229)</f>
+        <v>28</v>
+      </c>
+      <c r="K216" s="2">
+        <f>SUM(E217:E228)</f>
+        <v>0</v>
+      </c>
+      <c r="L216" s="2">
+        <f>SUM(I216:K216)</f>
+        <v>77</v>
+      </c>
+      <c r="M216" s="15">
+        <f>L216*600</f>
+        <v>46200</v>
+      </c>
+      <c r="N216" s="15">
+        <v>30000</v>
+      </c>
+      <c r="O216" s="15">
+        <f>(M216-N216)/3</f>
+        <v>5400</v>
+      </c>
     </row>
     <row r="217" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B217" s="1">
@@ -9329,8 +9396,50 @@
         <v>4200</v>
       </c>
     </row>
+    <row r="227" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B227" s="1">
+        <v>45105</v>
+      </c>
+      <c r="C227">
+        <v>36</v>
+      </c>
+      <c r="F227" s="16">
+        <v>144000</v>
+      </c>
+    </row>
+    <row r="228" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B228" s="1">
+        <v>45106</v>
+      </c>
+      <c r="D228">
+        <v>24</v>
+      </c>
+      <c r="F228" s="16">
+        <v>103200</v>
+      </c>
+    </row>
+    <row r="229" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B229" s="1">
+        <v>45108</v>
+      </c>
+      <c r="C229">
+        <v>9</v>
+      </c>
+      <c r="F229" s="16">
+        <v>38700</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="H214:O214"/>
+    <mergeCell ref="B2:F4"/>
+    <mergeCell ref="I39:P39"/>
+    <mergeCell ref="I35:P35"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="I10:M10"/>
+    <mergeCell ref="I31:P31"/>
+    <mergeCell ref="I18:M18"/>
     <mergeCell ref="H209:O209"/>
     <mergeCell ref="H90:O90"/>
     <mergeCell ref="H86:O86"/>
@@ -9347,20 +9456,12 @@
     <mergeCell ref="H134:L134"/>
     <mergeCell ref="H194:O194"/>
     <mergeCell ref="H130:O130"/>
-    <mergeCell ref="B2:F4"/>
-    <mergeCell ref="I39:P39"/>
-    <mergeCell ref="I35:P35"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="I10:M10"/>
-    <mergeCell ref="I31:P31"/>
-    <mergeCell ref="I18:M18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="K33 J37 K41 J45 J49:K49 M49 J8 J20 M20 J88:K88 I92 I96:J96 K92 I100:J100 J104 L104 I120:J120 J124 J128 I132 I136 L136 I196:J196 I201 K201 I206:J206 I211" formulaRange="1"/>
+    <ignoredError sqref="K33 J37 K41 J45 J49:K49 M49 J8 J20 M20 J88:K88 I92 I96:J96 K92 I100:J100 J104 L104 I120:J120 J124 J128 I132 I136 L136 I196:J196 I201 K201 I206:J206 I211 I216" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
   <tableParts count="1">

</xml_diff>